<commit_message>
updating state emissions summary output
</commit_message>
<xml_diff>
--- a/state_fact_sheets/data/modified/il_naics_emissions_percentages_2023.xlsx
+++ b/state_fact_sheets/data/modified/il_naics_emissions_percentages_2023.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -360,31 +360,31 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>naics_code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>co2e_total</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>percent_of_total</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>sector</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>co2e_total</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>percent_of_total</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Other</t>
-        </is>
-      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Other Manufacturing</t>
@@ -396,11 +396,16 @@
       <c r="D2">
         <v>31.92</v>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Food and Beverage</t>
+          <t>311611</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -414,11 +419,16 @@
       <c r="D3">
         <v>0.8</v>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Food and Beverage</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Food and Beverage</t>
+          <t>312140</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -432,11 +442,16 @@
       <c r="D4">
         <v>1.08</v>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Food and Beverage</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Food and Beverage</t>
+          <t>311225</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -450,11 +465,16 @@
       <c r="D5">
         <v>0.29</v>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Food and Beverage</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Food and Beverage</t>
+          <t>311224</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -468,11 +488,16 @@
       <c r="D6">
         <v>1.68</v>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Food and Beverage</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Food and Beverage</t>
+          <t>311221</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -486,11 +511,16 @@
       <c r="D7">
         <v>33.75</v>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Food and Beverage</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325199</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -504,11 +534,16 @@
       <c r="D8">
         <v>0.65</v>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325998</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -522,11 +557,16 @@
       <c r="D9">
         <v>4.18</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325414</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -540,11 +580,16 @@
       <c r="D10">
         <v>0.33</v>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325194</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -558,11 +603,16 @@
       <c r="D11">
         <v>0.73</v>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325193</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -576,11 +626,16 @@
       <c r="D12">
         <v>11.84</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325120</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -594,11 +649,16 @@
       <c r="D13">
         <v>3.51</v>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325411</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -612,11 +672,16 @@
       <c r="D14">
         <v>0.25</v>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325311</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -630,11 +695,16 @@
       <c r="D15">
         <v>5.3</v>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325180</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -648,16 +718,21 @@
       <c r="D16">
         <v>0.45</v>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325613</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Other Manufacturing</t>
+          <t>Other Chemicals Manufacturing</t>
         </is>
       </c>
       <c r="C17">
@@ -666,11 +741,16 @@
       <c r="D17">
         <v>0.86</v>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325110</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -684,11 +764,16 @@
       <c r="D18">
         <v>2.1</v>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Chemicals</t>
+          <t>325211</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -701,6 +786,11 @@
       </c>
       <c r="D19">
         <v>0.3</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Chemicals</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>